<commit_message>
finalización login, formulario principal
</commit_message>
<xml_diff>
--- a/doc/Glosario.xlsx
+++ b/doc/Glosario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\victor\gitmio\CleverHelpDesk\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3442B232-8B1E-41E2-8CD7-3C3593AB0A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A3E4A0-C571-4450-9D64-0106E0629FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1116702B-8BD7-4855-B7AA-5AF5D1E7FCB3}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{1116702B-8BD7-4855-B7AA-5AF5D1E7FCB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Termino</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Multi-Plataforma</t>
+  </si>
+  <si>
+    <t>JWT</t>
+  </si>
+  <si>
+    <t>TOKEN</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA61A460-463D-46B0-B79E-A18376DC3A66}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
@@ -617,6 +623,16 @@
         <v>24</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
lo que faltaba por subir ;-)
</commit_message>
<xml_diff>
--- a/doc/Glosario.xlsx
+++ b/doc/Glosario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\victor\gitmio\CleverHelpDesk\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DF4908-E7BE-4BF4-ADC0-80AE0055907F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEBBC88-67A9-4D3F-82D2-A5831A9FBDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1116702B-8BD7-4855-B7AA-5AF5D1E7FCB3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1116702B-8BD7-4855-B7AA-5AF5D1E7FCB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Termino</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">framework </t>
   </si>
 </sst>
 </file>
@@ -539,9 +542,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA61A460-463D-46B0-B79E-A18376DC3A66}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -728,6 +731,11 @@
         <v>37</v>
       </c>
     </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>